<commit_message>
Se crea el usuario root y se carga empresas por excel
</commit_message>
<xml_diff>
--- a/classes/production/springboot-auth-updated/data/datamonitorear/sunsol.xlsx
+++ b/classes/production/springboot-auth-updated/data/datamonitorear/sunsol.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="5"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="divisiónTerritorial" sheetId="1" state="visible" r:id="rId2"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="274" uniqueCount="111">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="276" uniqueCount="113">
   <si>
     <t xml:space="preserve">CodigoRaizNivel_T</t>
   </si>
@@ -339,10 +339,16 @@
     <t xml:space="preserve">name</t>
   </si>
   <si>
+    <t xml:space="preserve">email</t>
+  </si>
+  <si>
     <t xml:space="preserve">E0001</t>
   </si>
   <si>
     <t xml:space="preserve">Sun Sol</t>
+  </si>
+  <si>
+    <t xml:space="preserve">solelena@hotmail.de</t>
   </si>
   <si>
     <t xml:space="preserve">Simon Alberto</t>
@@ -1895,16 +1901,16 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:B1048576"/>
+  <dimension ref="A1:C1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C8" activeCellId="0" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="1" style="0" width="22.67"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="3" style="0" width="8.22"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="3" style="0" width="8.21"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1914,17 +1920,26 @@
       <c r="B1" s="1" t="s">
         <v>103</v>
       </c>
+      <c r="C1" s="0" t="s">
+        <v>104</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>105</v>
+        <v>106</v>
+      </c>
+      <c r="C2" s="0" t="s">
+        <v>107</v>
       </c>
     </row>
     <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="C2" r:id="rId1" display="solelena@hotmail.de"/>
+  </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
   <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
@@ -1942,7 +1957,7 @@
   </sheetPr>
   <dimension ref="A1:D1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="C3" activeCellId="0" sqref="C3"/>
     </sheetView>
   </sheetViews>
@@ -1971,13 +1986,13 @@
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="4" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>108</v>
+        <v>110</v>
       </c>
       <c r="D2" s="3" t="s">
         <v>95</v>
@@ -1985,13 +2000,13 @@
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="4" t="s">
+        <v>111</v>
+      </c>
+      <c r="B3" s="4" t="s">
         <v>109</v>
       </c>
-      <c r="B3" s="4" t="s">
-        <v>107</v>
-      </c>
       <c r="C3" s="4" t="s">
-        <v>110</v>
+        <v>112</v>
       </c>
       <c r="D3" s="3" t="s">
         <v>94</v>

</xml_diff>